<commit_message>
hkc-caculator version 0.8 beta,change the way of showing data
fixed:can not show more than two files at the same time
</commit_message>
<xml_diff>
--- a/database/hkcdatabase/false-data/ads02-430fd (1).xlsx
+++ b/database/hkcdatabase/false-data/ads02-430fd (1).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24225" windowHeight="12540"/>
+    <workbookView windowWidth="24225" windowHeight="11940"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,8 +41,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -56,7 +56,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -69,22 +92,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -98,6 +116,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -106,21 +139,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -129,6 +147,50 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -136,70 +198,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -208,37 +208,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -250,139 +382,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -405,38 +411,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -467,9 +443,35 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -489,13 +491,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -507,10 +513,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -519,141 +525,144 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1004,13 +1013,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
   <cols>
     <col min="4" max="4" width="9.375"/>
   </cols>
@@ -1023,7 +1032,7 @@
         <v>1</v>
       </c>
       <c r="D1">
-        <v>20220301</v>
+        <v>20220302</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1110,7 +1119,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1123,6 +1132,7 @@
       <c r="D8" s="1">
         <v>32</v>
       </c>
+      <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9">

</xml_diff>